<commit_message>
added commands, worked on lots of others stuff
</commit_message>
<xml_diff>
--- a/py Sorting and Comparing/testemails_Duplicates.xlsx
+++ b/py Sorting and Comparing/testemails_Duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work_Share_cloud\VBALAB_data\Teacher Repository\Teacher Email Managment\py Sorting and Comparing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\codin\PycharmProjects\EmailManagement\py Sorting and Comparing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD8C224-C33A-4CB1-A079-EC4036471366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906206F7-7818-4B71-B028-4DAD3B89AC38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="13905" windowWidth="20910" windowHeight="13740" xr2:uid="{9D30211D-81D0-4F62-BFBB-7E4FDF899D2C}"/>
+    <workbookView xWindow="18270" yWindow="22170" windowWidth="21600" windowHeight="11475" xr2:uid="{9D30211D-81D0-4F62-BFBB-7E4FDF899D2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>181884@dadeschools.net</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>2ndEmail</t>
-  </si>
-  <si>
     <t>role</t>
   </si>
   <si>
@@ -118,6 +115,15 @@
   </si>
   <si>
     <t>eat@gmail.com</t>
+  </si>
+  <si>
+    <t>Contact2</t>
+  </si>
+  <si>
+    <t>akillingbeck@gmail.com</t>
+  </si>
+  <si>
+    <t>arnold</t>
   </si>
 </sst>
 </file>
@@ -520,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8350FABE-1506-4F55-864C-AC85584203E8}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,10 +551,10 @@
         <v>20</v>
       </c>
       <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -556,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -585,10 +591,10 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -596,10 +602,10 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -607,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -615,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -655,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -663,7 +669,7 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -696,6 +702,14 @@
       </c>
       <c r="C19" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>